<commit_message>
before framework update - 5/6
</commit_message>
<xml_diff>
--- a/data/ItemList.xlsx
+++ b/data/ItemList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yukina\Documents\GitHub\Critical-Story\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C6C0E76-BEC8-4556-80CB-690F79D74C10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{818A2880-5E8B-4DB5-886B-A77E23A2C01E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="428">
   <si>
     <t>ItemId</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -884,10 +884,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>200</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PurifyPotion</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1039,10 +1035,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Deal &lt;purple&gt;magic damage&lt;/font&gt; to the enemy and inflict &lt;red&gt;Burn&lt;/font&gt; for &lt;blue&gt;2 TURN&lt;/font&gt;, cost &lt;blue&gt;40% TP&lt;/font&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Fire a ball towards enemy, mark an area under it, which deals &lt;purple&gt;magic damage&lt;/font&gt;, cost &lt;blue&gt;50% TP&lt;/font&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1051,10 +1043,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Strike down a beam to deal &lt;purple&gt;magic damage&lt;/font&gt; to the enemy and inflict &lt;red&gt;CHAOS&lt;/font&gt; for &lt;blue&gt;1 TURN&lt;/font&gt;, costs &lt;blue&gt;60% TP&lt;/font&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Slash out a blade of pure raw physical energy that deals &lt;red&gt;physical damage&lt;/font&gt;, cost &lt;blue&gt;50% TP&lt;/font&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1107,14 +1095,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Endurance</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4824422041</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Enrage</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1215,22 +1195,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ModusShift</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4824414597</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MorphStrike</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Morph Strike</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>4851324727</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1283,10 +1247,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>kitty, you can have this burger</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>17367034811</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1338,38 +1298,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ThrowingDagger</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Throwing Dagger</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4828797495</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ThrowingKnife</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Throwing Knife</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4851323883</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ThyrsusQuillDagger</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Thyrsus Quill Dagger</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>4820498554</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1402,22 +1330,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CHANCE! Break the shield!</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5,4,3,2,1!</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CRITICAL! After all, it's critical story</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Modus Shift</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>&lt;orange&gt;+50 Shield&lt;/font&gt;, restore &lt;blue&gt;10% more TP&lt;/font&gt; for every attack</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1466,7 +1378,295 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Hava a &lt;blue&gt;30% chance&lt;/font&gt; to cause random &lt;red&gt;debuff&lt;/font&gt; to enemy when you land an attack</t>
+    <t>Strike down a beam to deal &lt;purple&gt;magic damage&lt;/font&gt; to the enemy and inflict &lt;red&gt;BURN&lt;/font&gt; for &lt;blue&gt;1 TURN&lt;/font&gt;, costs &lt;blue&gt;60% TP&lt;/font&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A spell that is famously used for breaking hard carapaces or metals</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Powerful weapons created to break through the hardest defenses</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A scroll which enhances ones ability to obtain a critical hit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deals &lt;red&gt;physical damage&lt;/font&gt; to the enemy regardless of defense, costs &lt;blue&gt;30% TP&lt;/font&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deals &lt;red&gt;3X physical damage&lt;/font&gt; to the enemy, costs &lt;blue&gt;40% TP&lt;/font&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A skill that calls out protection from the gods</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;blue&gt;+90% Defense&lt;/font&gt; for &lt;blue&gt;1 TURN&lt;/font&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EndurancePotion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Endurance Potion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2970818737</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A skill passed down from the great barbarians, use it wisely</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;red&gt;+50% Min Damage and +100% Max Damage&lt;/font&gt; for &lt;blue&gt;1 TURN&lt;/blue&gt;, costs &lt;blue&gt;40% TP&lt;/font&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;yellow&gt;+5% Critical Chance&lt;/font&gt; for &lt;blue&gt;1 TURN&lt;/font&gt;, costs &lt;blue&gt;30% TP&lt;/font&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"If you wish to hide in the darkness, then the darkness will hide in you" -Shard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Slash out a sword that deals &lt;red&gt;physical damage&lt;/font&gt;, cost &lt;blue&gt;60% TP&lt;/font&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A spell that creates a powerful mini explosion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unleashes a powerful explosion, &lt;blue&gt;costs 80% TP&lt;/font&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cheap effective daggers made from the core of an Ice Slime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deals &lt;red&gt;physical damage&lt;/font&gt; and inflict &lt;blue&gt;FREEZE&lt;/font&gt;, costs &lt;blue&gt;50% TP&lt;/font&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A scroll that allows you to cast a chilling flash freeze</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deals &lt;red&gt;magic damage&lt;/font&gt; and inflict &lt;blue&gt;FREEZE&lt;/font&gt;, costs &lt;blue&gt;50% TP&lt;/font&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tastes like honey</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Used for &lt;purple&gt;Alchemy&lt;/font&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sweet treats from the north that came from slimes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A spell that can heal you</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Recover &lt;green&gt;90% Health&lt;/font&gt;, costs &lt;blue&gt;70% TP&lt;/font&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Recover &lt;green&gt;25% Health&lt;/font&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Warrios use this ability to quickly power himself</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;red&gt;+100% Max Damage&lt;/font&gt; for &lt;blue&gt;3 TURNS&lt;/font&gt;, and recover &lt;green&gt;70% Health&lt;/font&gt;, costs &lt;blue&gt;70% TP&lt;/font&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gain &lt;blue&gt;10% Defense&lt;/font&gt; for &lt;blue&gt;2 TURNS&lt;/font&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deal &lt;purple&gt;magic damage&lt;/font&gt; to the enemy and inflict &lt;red&gt;Burn&lt;/font&gt; for &lt;blue&gt;2 TURNS&lt;/font&gt;, cost &lt;blue&gt;40% TP&lt;/font&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A skill that allows you to preserve your own life energy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Recover &lt;green&gt;70% Health&lt;/font&gt;, costs &lt;blue&gt;50% TP&lt;/font&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fire an edgy laser to obliterate your foes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fire a devastating laser that deals huge &lt;purple&gt;magic damage&lt;/font&gt; to the enemy, costs &lt;blue&gt;70% TP&lt;/font&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Made from the quills of wolves and foxes, making it lightweight but deadly</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;red&gt;+30 Max Damage&lt;/font&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Only achieved by the worthy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Slash through reality dealing &lt;red&gt;perfectage physical damage&lt;/font&gt; on the enemy, costs &lt;blue&gt;60% TP&lt;/font&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I thought only bugs had souls</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Conjure a &lt;purple&gt;magical blast&lt;/font&gt; to the enemy, costs &lt;blue&gt;50% TP&lt;/font&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kitty, you can have this burger. Smells yummy, I wonder whats the recipe?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Recover &lt;green&gt;100% Health&lt;/font&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A spell that creates powerful barrage of different spells</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unleashes a barrage of random unknown spells that &lt;blue&gt;costs 100% TP&lt;/font&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A special ability that shoots out a star</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shoot out a star that &lt;blue&gt;STUNS&lt;/font&gt; a target, costs &lt;blue&gt;40% TP&lt;/font&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A skill allowing the user to become that of the earth, refining defense</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gain &lt;blue&gt;50% Defense&lt;/font&gt; for &lt;blue&gt;2 TURNS&lt;/font&gt;, but reduce &lt;blue&gt;50% Speed&lt;/font&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A skill that allows the user become stronger</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;red&gt;+20 Damage&lt;/font&gt; for &lt;blue&gt;5 TURNS&lt;/font&gt;, costs &lt;blue&gt;10% TP&lt;/font&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A spell that casts a ball of darkness</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deals tremendous &lt;purple&gt;magic damage&lt;/font&gt; to the enemy, costs &lt;blue&gt;40% TP&lt;/blue&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lux</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A spell that casts a ball of light</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4820492332</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deals heavy &lt;purple&gt;magic damage&lt;/font&gt; to the enemy, costs &lt;blue&gt;35% TP&lt;/blue&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Axes made for throwing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deals &lt;red&gt;Max Damage&lt;/font&gt; to the enemy, costs &lt;blue&gt;30% TP&lt;/font&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A spell that makes the target weak</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Casts a &lt;purple&gt;weakness&lt;/font&gt; debuff onto the enemy for &lt;blue&gt;3 TURNS&lt;/font&gt;, costs &lt;blue&gt;30% TP&lt;/font&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Little spirits are attracted to you</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Summons a fireball that homes onto the target, dealing &lt;purple&gt;magical damage&lt;/font&gt; and inflict &lt;red&gt;BURN&lt;/font&gt; for &lt;blue&gt;1 TURN&lt;/font&gt;. After every use, increase fireball count by 1 for the rest of the battle, up to 3. Costs &lt;blue&gt;50% TP&lt;/font&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SharpenerRock</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sharpener Rock</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A flat rock used to sharpen blades</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;yellow&gt;+10% Critical Chance&lt;/font&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2965825317</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Have a &lt;blue&gt;30% chance&lt;/font&gt; to cause random &lt;red&gt;debuff&lt;/font&gt; to enemy when you land an attack</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1861,11 +2061,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L88"/>
+  <dimension ref="A1:L85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F84" sqref="F84"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
@@ -1916,7 +2116,7 @@
         <v>7</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>216</v>
@@ -1939,7 +2139,7 @@
         <v>118</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>166</v>
@@ -1977,7 +2177,7 @@
         <v>119</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>167</v>
@@ -2015,10 +2215,10 @@
         <v>120</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>116</v>
@@ -2041,7 +2241,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>370</v>
+        <v>348</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>33</v>
@@ -2053,7 +2253,7 @@
         <v>120</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>168</v>
@@ -2076,10 +2276,10 @@
     </row>
     <row r="6" spans="1:12" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>368</v>
+        <v>346</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>369</v>
+        <v>347</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>33</v>
@@ -2091,10 +2291,10 @@
         <v>120</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>371</v>
+        <v>349</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>372</v>
+        <v>350</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>116</v>
@@ -2129,7 +2329,7 @@
         <v>120</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>169</v>
@@ -2138,7 +2338,7 @@
         <v>116</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>115</v>
@@ -2152,10 +2352,10 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>225</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>33</v>
@@ -2167,10 +2367,10 @@
         <v>120</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>116</v>
@@ -2205,7 +2405,7 @@
         <v>121</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>170</v>
@@ -2243,7 +2443,7 @@
         <v>122</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>171</v>
@@ -2281,7 +2481,7 @@
         <v>123</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>172</v>
@@ -2319,7 +2519,7 @@
         <v>124</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>173</v>
@@ -2357,7 +2557,7 @@
         <v>125</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>270</v>
+        <v>388</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>174</v>
@@ -2372,7 +2572,7 @@
         <v>116</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L13" s="4">
         <v>0</v>
@@ -2395,7 +2595,7 @@
         <v>126</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>175</v>
@@ -2410,7 +2610,7 @@
         <v>116</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="L14" s="4">
         <v>0</v>
@@ -2433,7 +2633,7 @@
         <v>127</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>273</v>
+        <v>355</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>176</v>
@@ -2448,7 +2648,7 @@
         <v>116</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="L15" s="4">
         <v>0</v>
@@ -2471,7 +2671,7 @@
         <v>128</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>177</v>
@@ -2509,10 +2709,10 @@
         <v>129</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>367</v>
+        <v>345</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>115</v>
@@ -2547,7 +2747,7 @@
         <v>130</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>178</v>
@@ -2585,7 +2785,7 @@
         <v>131</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>179</v>
@@ -2623,7 +2823,7 @@
         <v>132</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>180</v>
@@ -2661,7 +2861,7 @@
         <v>133</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>181</v>
@@ -2699,7 +2899,7 @@
         <v>134</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>182</v>
@@ -2737,10 +2937,10 @@
         <v>135</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>115</v>
@@ -2775,7 +2975,7 @@
         <v>136</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>183</v>
@@ -2813,7 +3013,7 @@
         <v>137</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>184</v>
@@ -2851,7 +3051,7 @@
         <v>138</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>185</v>
@@ -2889,7 +3089,7 @@
         <v>139</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>187</v>
@@ -2927,7 +3127,7 @@
         <v>140</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>366</v>
+        <v>344</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>186</v>
@@ -2965,7 +3165,7 @@
         <v>141</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>188</v>
@@ -3003,7 +3203,7 @@
         <v>142</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>189</v>
@@ -3041,7 +3241,7 @@
         <v>143</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>190</v>
@@ -3079,7 +3279,7 @@
         <v>144</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>191</v>
@@ -3117,7 +3317,7 @@
         <v>145</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>192</v>
@@ -3155,7 +3355,7 @@
         <v>146</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>193</v>
@@ -3193,7 +3393,7 @@
         <v>147</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>194</v>
@@ -3231,7 +3431,7 @@
         <v>148</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>195</v>
@@ -3269,7 +3469,7 @@
         <v>149</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>196</v>
@@ -3307,7 +3507,7 @@
         <v>150</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>197</v>
@@ -3342,10 +3542,10 @@
         <v>114</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>198</v>
@@ -3383,7 +3583,7 @@
         <v>151</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>199</v>
@@ -3421,7 +3621,7 @@
         <v>152</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>365</v>
+        <v>343</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>200</v>
@@ -3459,7 +3659,7 @@
         <v>153</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>201</v>
@@ -3497,7 +3697,7 @@
         <v>154</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>202</v>
@@ -3535,7 +3735,7 @@
         <v>155</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>203</v>
@@ -3573,7 +3773,7 @@
         <v>156</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>204</v>
@@ -3611,7 +3811,7 @@
         <v>157</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>205</v>
@@ -3649,7 +3849,7 @@
         <v>158</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>206</v>
@@ -3687,7 +3887,7 @@
         <v>159</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>207</v>
@@ -3725,7 +3925,7 @@
         <v>160</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>208</v>
@@ -3763,7 +3963,7 @@
         <v>161</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>209</v>
@@ -3801,7 +4001,7 @@
         <v>162</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>210</v>
@@ -3839,7 +4039,7 @@
         <v>163</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>211</v>
@@ -3877,7 +4077,7 @@
         <v>164</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>212</v>
@@ -3915,7 +4115,7 @@
         <v>165</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>213</v>
@@ -3936,12 +4136,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>33</v>
@@ -3950,10 +4150,13 @@
         <v>34</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>361</v>
+        <v>356</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>359</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="H55" s="2" t="s">
         <v>115</v>
@@ -3965,18 +4168,18 @@
         <v>116</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>117</v>
+        <v>367</v>
       </c>
       <c r="L55" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>33</v>
@@ -3985,10 +4188,13 @@
         <v>34</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>362</v>
+        <v>357</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>360</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="H56" s="2" t="s">
         <v>115</v>
@@ -4000,18 +4206,18 @@
         <v>116</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>117</v>
+        <v>367</v>
       </c>
       <c r="L56" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>33</v>
@@ -4020,10 +4226,13 @@
         <v>35</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>363</v>
+        <v>358</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>370</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="H57" s="2" t="s">
         <v>115</v>
@@ -4035,18 +4244,18 @@
         <v>116</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>117</v>
+        <v>367</v>
       </c>
       <c r="L57" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>33</v>
@@ -4054,8 +4263,14 @@
       <c r="D58" s="2" t="s">
         <v>114</v>
       </c>
+      <c r="E58" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>362</v>
+      </c>
       <c r="G58" s="2" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>115</v>
@@ -4067,18 +4282,18 @@
         <v>116</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>117</v>
+        <v>367</v>
       </c>
       <c r="L58" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>287</v>
+        <v>363</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>287</v>
+        <v>364</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>33</v>
@@ -4086,31 +4301,37 @@
       <c r="D59" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="E59" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>387</v>
+      </c>
       <c r="G59" s="2" t="s">
-        <v>288</v>
+        <v>365</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I59" s="2" t="s">
         <v>218</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K59" s="2" t="s">
         <v>117</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>33</v>
@@ -4118,8 +4339,14 @@
       <c r="D60" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="E60" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>369</v>
+      </c>
       <c r="G60" s="2" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="H60" s="2" t="s">
         <v>115</v>
@@ -4131,18 +4358,18 @@
         <v>116</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>117</v>
+        <v>367</v>
       </c>
       <c r="L60" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>33</v>
@@ -4150,8 +4377,14 @@
       <c r="D61" s="2" t="s">
         <v>114</v>
       </c>
+      <c r="E61" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>372</v>
+      </c>
       <c r="G61" s="2" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="H61" s="2" t="s">
         <v>115</v>
@@ -4163,27 +4396,33 @@
         <v>116</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>117</v>
+        <v>367</v>
       </c>
       <c r="L61" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>35</v>
+        <v>114</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>374</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="H62" s="2" t="s">
         <v>115</v>
@@ -4195,18 +4434,18 @@
         <v>116</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>117</v>
+        <v>367</v>
       </c>
       <c r="L62" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>33</v>
@@ -4214,8 +4453,14 @@
       <c r="D63" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="E63" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>376</v>
+      </c>
       <c r="G63" s="2" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="H63" s="2" t="s">
         <v>115</v>
@@ -4227,27 +4472,33 @@
         <v>116</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>117</v>
+        <v>367</v>
       </c>
       <c r="L63" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>114</v>
+        <v>35</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>378</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="H64" s="2" t="s">
         <v>115</v>
@@ -4259,7 +4510,7 @@
         <v>116</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>117</v>
+        <v>367</v>
       </c>
       <c r="L64" s="2" t="s">
         <v>117</v>
@@ -4267,19 +4518,25 @@
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>33</v>
+        <v>112</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="E65" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>380</v>
+      </c>
       <c r="G65" s="2" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="H65" s="2" t="s">
         <v>116</v>
@@ -4297,12 +4554,12 @@
         <v>117</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>33</v>
@@ -4310,8 +4567,14 @@
       <c r="D66" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="E66" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>383</v>
+      </c>
       <c r="G66" s="2" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="H66" s="2" t="s">
         <v>115</v>
@@ -4323,7 +4586,7 @@
         <v>116</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>117</v>
+        <v>367</v>
       </c>
       <c r="L66" s="2" t="s">
         <v>117</v>
@@ -4331,10 +4594,10 @@
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>33</v>
@@ -4342,8 +4605,14 @@
       <c r="D67" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="E67" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>384</v>
+      </c>
       <c r="G67" s="2" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="H67" s="2" t="s">
         <v>116</v>
@@ -4361,12 +4630,12 @@
         <v>117</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" ht="62.4" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>33</v>
@@ -4374,8 +4643,14 @@
       <c r="D68" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="E68" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>386</v>
+      </c>
       <c r="G68" s="2" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="H68" s="2" t="s">
         <v>115</v>
@@ -4387,18 +4662,18 @@
         <v>116</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>117</v>
+        <v>367</v>
       </c>
       <c r="L68" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>33</v>
@@ -4406,8 +4681,14 @@
       <c r="D69" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="E69" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>390</v>
+      </c>
       <c r="G69" s="2" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="H69" s="2" t="s">
         <v>115</v>
@@ -4419,18 +4700,18 @@
         <v>116</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>117</v>
+        <v>367</v>
       </c>
       <c r="L69" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>364</v>
+        <v>310</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>33</v>
@@ -4438,8 +4719,14 @@
       <c r="D70" s="2" t="s">
         <v>114</v>
       </c>
+      <c r="E70" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>392</v>
+      </c>
       <c r="G70" s="2" t="s">
-        <v>282</v>
+        <v>309</v>
       </c>
       <c r="H70" s="2" t="s">
         <v>115</v>
@@ -4451,27 +4738,33 @@
         <v>116</v>
       </c>
       <c r="K70" s="2" t="s">
-        <v>117</v>
+        <v>367</v>
       </c>
       <c r="L70" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>114</v>
+        <v>34</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>394</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="H71" s="2" t="s">
         <v>115</v>
@@ -4483,27 +4776,33 @@
         <v>116</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>117</v>
+        <v>367</v>
       </c>
       <c r="L71" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>114</v>
+        <v>35</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>396</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="H72" s="2" t="s">
         <v>115</v>
@@ -4515,27 +4814,33 @@
         <v>116</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>117</v>
+        <v>367</v>
       </c>
       <c r="L72" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>398</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>322</v>
+        <v>279</v>
       </c>
       <c r="H73" s="2" t="s">
         <v>115</v>
@@ -4547,50 +4852,56 @@
         <v>116</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>117</v>
+        <v>367</v>
       </c>
       <c r="L73" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>400</v>
       </c>
       <c r="G74" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="I74" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="J74" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="K74" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="L74" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" ht="31.2" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="H74" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="I74" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="J74" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="K74" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="L74" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
-        <v>326</v>
-      </c>
       <c r="B75" s="2" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>33</v>
@@ -4598,8 +4909,14 @@
       <c r="D75" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="E75" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>403</v>
+      </c>
       <c r="G75" s="2" t="s">
-        <v>282</v>
+        <v>322</v>
       </c>
       <c r="H75" s="2" t="s">
         <v>115</v>
@@ -4611,53 +4928,56 @@
         <v>116</v>
       </c>
       <c r="K75" s="2" t="s">
-        <v>117</v>
+        <v>367</v>
       </c>
       <c r="L75" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>331</v>
+        <v>404</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>405</v>
       </c>
       <c r="G76" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I76" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="J76" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="K76" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="L76" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" ht="46.8" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="H76" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="I76" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="J76" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="K76" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="L76" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
-        <v>333</v>
-      </c>
       <c r="B77" s="2" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>33</v>
@@ -4665,8 +4985,14 @@
       <c r="D77" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="E77" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>407</v>
+      </c>
       <c r="G77" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="H77" s="2" t="s">
         <v>115</v>
@@ -4678,27 +5004,33 @@
         <v>116</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>117</v>
+        <v>367</v>
       </c>
       <c r="L77" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>409</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="H78" s="2" t="s">
         <v>115</v>
@@ -4710,18 +5042,18 @@
         <v>116</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>117</v>
+        <v>367</v>
       </c>
       <c r="L78" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>33</v>
@@ -4729,8 +5061,14 @@
       <c r="D79" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="E79" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>411</v>
+      </c>
       <c r="G79" s="2" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="H79" s="2" t="s">
         <v>115</v>
@@ -4742,27 +5080,33 @@
         <v>116</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>117</v>
+        <v>367</v>
       </c>
       <c r="L79" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>342</v>
+        <v>412</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>342</v>
+        <v>412</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>415</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>341</v>
+        <v>414</v>
       </c>
       <c r="H80" s="2" t="s">
         <v>115</v>
@@ -4774,18 +5118,18 @@
         <v>116</v>
       </c>
       <c r="K80" s="2" t="s">
-        <v>117</v>
+        <v>367</v>
       </c>
       <c r="L80" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>33</v>
@@ -4793,8 +5137,14 @@
       <c r="D81" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="E81" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>417</v>
+      </c>
       <c r="G81" s="2" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="H81" s="2" t="s">
         <v>115</v>
@@ -4806,18 +5156,18 @@
         <v>116</v>
       </c>
       <c r="K81" s="2" t="s">
-        <v>117</v>
+        <v>367</v>
       </c>
       <c r="L81" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" ht="62.4" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>33</v>
@@ -4825,8 +5175,14 @@
       <c r="D82" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="E82" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>419</v>
+      </c>
       <c r="G82" s="2" t="s">
-        <v>322</v>
+        <v>337</v>
       </c>
       <c r="H82" s="2" t="s">
         <v>115</v>
@@ -4838,27 +5194,33 @@
         <v>116</v>
       </c>
       <c r="K82" s="2" t="s">
-        <v>117</v>
+        <v>367</v>
       </c>
       <c r="L82" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" ht="124.8" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>421</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="H83" s="2" t="s">
         <v>115</v>
@@ -4870,175 +5232,85 @@
         <v>116</v>
       </c>
       <c r="K83" s="2" t="s">
-        <v>117</v>
+        <v>367</v>
       </c>
       <c r="L83" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="84" spans="1:12" ht="31.2" x14ac:dyDescent="0.25">
-      <c r="A84" s="2" t="s">
+    <row r="84" spans="1:12" ht="46.8" x14ac:dyDescent="0.25">
+      <c r="A84" s="6" t="s">
         <v>351</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="C84" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D84" s="2" t="s">
+      <c r="D84" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G84" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="H84" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="I84" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="J84" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="K84" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="L84" s="2" t="s">
+      <c r="E84" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="G84" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="H84" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="I84" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="J84" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="K84" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="L84" s="6" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="s">
-        <v>354</v>
+      <c r="A85" s="6" t="s">
+        <v>422</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G85" s="2" t="s">
-        <v>353</v>
-      </c>
-      <c r="H85" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="I85" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="J85" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="K85" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="L85" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D86" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D85" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G86" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="H86" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="I86" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="J86" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="K86" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="L86" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A87" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G87" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="H87" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="I87" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="J87" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="K87" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="L87" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" ht="46.8" x14ac:dyDescent="0.25">
-      <c r="A88" s="6" t="s">
-        <v>373</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="C88" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D88" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E88" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="F88" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="G88" s="6" t="s">
-        <v>375</v>
-      </c>
-      <c r="H88" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="I88" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="J88" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="K88" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="L88" s="6" t="s">
+      <c r="E85" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="G85" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="H85" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="I85" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="J85" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="K85" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="L85" s="6" t="s">
         <v>117</v>
       </c>
     </row>

</xml_diff>